<commit_message>
updated libraries, advanced formattig template , sync job
</commit_message>
<xml_diff>
--- a/HydroServerTools/Templates/Advanced Formatting Template.xlsx
+++ b/HydroServerTools/Templates/Advanced Formatting Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbrazil\Documents\Publishing Process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Azure-Hydroservertools\HydroServerTools\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5B4EB2-28BD-430C-A44C-C4C17C4274AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6570" tabRatio="751" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="751" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="30" r:id="rId1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="249">
   <si>
     <t>Field Name</t>
   </si>
@@ -1095,7 +1096,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1794,20 +1795,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1825,6 +1814,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2205,28 +2206,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="30" t="s">
         <v>103</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="31" t="s">
         <v>149</v>
       </c>
@@ -2243,38 +2244,38 @@
       <c r="M3" s="31"/>
       <c r="N3" s="31"/>
     </row>
-    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="B5" s="32" t="s">
         <v>231</v>
       </c>
       <c r="C5" s="32"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
@@ -2288,7 +2289,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" s="29" t="s">
         <v>101</v>
       </c>
@@ -2302,7 +2303,7 @@
       <c r="J16" s="29"/>
       <c r="K16" s="29"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
@@ -2316,7 +2317,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>102</v>
       </c>
@@ -2330,17 +2331,17 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="22" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="33" t="s">
         <v>100</v>
       </c>
@@ -2354,7 +2355,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="29" t="s">
         <v>110</v>
       </c>
@@ -2369,7 +2370,7 @@
       <c r="K22" s="29"/>
       <c r="L22" s="29"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="29" t="s">
         <v>232</v>
       </c>
@@ -2383,7 +2384,7 @@
       <c r="J23" s="29"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
         <v>230</v>
       </c>
@@ -2396,7 +2397,7 @@
       <c r="I26" s="24"/>
       <c r="J26" s="25"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="26"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -2424,33 +2425,33 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.44140625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2556,7 +2557,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2609,7 +2610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="300" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -2662,7 +2663,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2722,22 +2723,22 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2765,7 +2766,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2779,7 +2780,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -2793,7 +2794,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2813,21 +2814,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2838,7 +2839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2849,7 +2850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
@@ -2860,7 +2861,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
@@ -2871,7 +2872,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2888,21 +2889,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2913,7 +2914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2924,7 +2925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -2946,7 +2947,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2963,20 +2964,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2987,7 +2988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2998,7 +2999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -3009,7 +3010,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
@@ -3020,7 +3021,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -3037,140 +3038,157 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>225</v>
+        <v>48</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="14" t="s">
         <v>228</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -3187,587 +3205,585 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" activeCellId="1" sqref="A12:P15 A20:P29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="41"/>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="44"/>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="37"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="40"/>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="42"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="42"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="42"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="42"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="43"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="43"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-    </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-    </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="42"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+    </row>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-    </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="44"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+    </row>
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-    </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="43"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+    </row>
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
-    </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="43"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
+    </row>
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="37"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="37"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-    </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="34"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="43"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
+      <c r="P27" s="34"/>
+    </row>
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="37"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
+      <c r="P28" s="34"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="43"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B24:P25"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B12:P13"/>
-    <mergeCell ref="B14:P15"/>
-    <mergeCell ref="B16:P17"/>
-    <mergeCell ref="B18:P19"/>
-    <mergeCell ref="B22:P23"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B26:P27"/>
     <mergeCell ref="B28:P29"/>
@@ -3784,39 +3800,41 @@
     <mergeCell ref="B6:P7"/>
     <mergeCell ref="B8:P9"/>
     <mergeCell ref="B10:P11"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B24:P25"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B12:P13"/>
+    <mergeCell ref="B14:P15"/>
+    <mergeCell ref="B16:P17"/>
+    <mergeCell ref="B18:P19"/>
+    <mergeCell ref="B22:P23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3857,7 +3875,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3898,7 +3916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -3939,7 +3957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -3980,7 +3998,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -4027,22 +4045,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4056,7 +4074,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -4070,7 +4088,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4084,7 +4102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4098,7 +4116,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -4119,33 +4137,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4195,7 +4213,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4245,7 +4263,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4292,7 +4310,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="13" customFormat="1" ht="210" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" s="13" customFormat="1" ht="172.8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4342,7 +4360,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -4395,28 +4413,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="12" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="12" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="65.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4472,7 +4490,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4528,7 +4546,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4584,7 +4602,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="13" customFormat="1" ht="150" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="13" customFormat="1" ht="129.6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4640,7 +4658,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -4681,7 +4699,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N6" t="s">
         <v>96</v>
       </c>
@@ -4705,20 +4723,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4732,7 +4750,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4746,7 +4764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4760,7 +4778,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -4774,7 +4792,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -4794,22 +4812,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4829,7 +4847,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -4849,7 +4867,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4869,7 +4887,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4889,7 +4907,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -4915,21 +4933,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4943,7 +4961,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4957,7 +4975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4971,7 +4989,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4985,7 +5003,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>